<commit_message>
New Filtwration api added
</commit_message>
<xml_diff>
--- a/Test Case sumary report.xlsx
+++ b/Test Case sumary report.xlsx
@@ -404,6 +404,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,15 +424,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,26 +731,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13"/>
+      <c r="A3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="16"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -796,21 +796,21 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
@@ -965,22 +965,22 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="15"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="13"/>
+      <c r="A23" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="16"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="14"/>
+      <c r="B24" s="17"/>
     </row>
     <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1023,21 +1023,21 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
@@ -1122,34 +1122,34 @@
       <c r="B36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="13">
         <v>1</v>
       </c>
-      <c r="E36" s="17">
-        <v>0</v>
-      </c>
-      <c r="F36" s="15" t="s">
+      <c r="E36" s="13">
+        <v>0</v>
+      </c>
+      <c r="F36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="11" t="s">
         <v>21</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I36" s="15">
+      <c r="I36" s="11">
         <v>400</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="11">
         <v>400</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="K36" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L36" s="15" t="s">
+      <c r="L36" s="11" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1157,57 +1157,57 @@
       <c r="A37" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="13">
         <v>1</v>
       </c>
-      <c r="E37" s="17">
-        <v>0</v>
-      </c>
-      <c r="F37" s="15" t="s">
+      <c r="E37" s="13">
+        <v>0</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H37" s="16" t="s">
+      <c r="H37" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="I37" s="15">
+      <c r="I37" s="11">
         <v>400</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="11">
         <v>400</v>
       </c>
-      <c r="K37" s="15" t="s">
+      <c r="K37" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="L37" s="15" t="s">
+      <c r="L37" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="12"/>
+      <c r="B40" s="15"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="13"/>
+      <c r="A42" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="16"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="14"/>
+      <c r="B43" s="17"/>
     </row>
     <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
@@ -1250,21 +1250,21 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
@@ -1419,22 +1419,22 @@
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B59" s="12"/>
+      <c r="B59" s="15"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="13"/>
+      <c r="A61" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="16"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="14"/>
+      <c r="B62" s="17"/>
     </row>
     <row r="63" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
@@ -1477,21 +1477,21 @@
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="11"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
@@ -1646,22 +1646,22 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
+      <c r="A77" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B77" s="12"/>
+      <c r="B77" s="15"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B79" s="13"/>
+      <c r="A79" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" s="16"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B80" s="14"/>
+      <c r="B80" s="17"/>
     </row>
     <row r="81" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
@@ -1704,21 +1704,21 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B87" s="11"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
-      <c r="L87" s="11"/>
-      <c r="M87" s="11"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
@@ -1874,26 +1874,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A12:M12"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A51:M51"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
     <mergeCell ref="A69:M69"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A79:B79"/>
     <mergeCell ref="A80:B80"/>
     <mergeCell ref="A87:M87"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A51:M51"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A32:M32"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A12:M12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>